<commit_message>
Improve column matching and scoring rule logic
- Prioritize annual target columns over semi-annual ones
- Exclude '半年度' columns when matching target and rule columns
- Improve baseline value extraction to handle score thresholds correctly
- Add ratio-based rule detection

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/processed_scorecard.xlsx
+++ b/processed_scorecard.xlsx
@@ -800,21 +800,21 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>0.68</t>
+          <t>0.65</t>
         </is>
       </c>
       <c r="P4" s="3" t="inlineStr">
         <is>
-          <t>P为指标实际值，0.85为目标值，0.68为底线值。
+          <t>P为指标实际值，0.85为目标值，0.65为底线值。
 1.若P≥0.85，得100分（满分）；
-2.若0.68&lt;P&lt;0.85，按线性比例计算，即：得分=60+(P-0.68)/(0.85-0.68)×(100-60)；
-3.若P=0.68，得60分（基础分）；
-4.若P&lt;0.68，得0分。</t>
+2.若0.65&lt;P&lt;0.85，按线性比例计算，即：得分=60+(P-0.65)/(0.85-0.65)×(100-60)；
+3.若P=0.65，得60分（基础分）；
+4.若P&lt;0.65，得0分。</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>人工校验</t>
+          <t>成功</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -888,21 +888,21 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>2.4</t>
+          <t>4</t>
         </is>
       </c>
       <c r="P5" s="3" t="inlineStr">
         <is>
-          <t>P为指标实际值，3为目标值，2.4为底线值。
-1.若P≥3，得100分（满分）；
-2.若2.4&lt;P&lt;3，按线性比例计算，即：得分=60+(P-2.4)/(3-2.4)×(100-60)；
-3.若P=2.4，得60分（基础分）；
-4.若P&lt;2.4，得0分。</t>
+          <t>P为指标实际值，6为目标值，4为底线值。
+1.若P≥6，得100分（满分）；
+2.若4&lt;P&lt;6，按线性比例计算，即：得分=60+(P-4)/(6-4)×(100-60)；
+3.若P=4，得60分（基础分）；
+4.若P&lt;4，得0分。</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>人工校验</t>
+          <t>成功</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -977,21 +977,21 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>0.76</t>
+          <t>0.8</t>
         </is>
       </c>
       <c r="P6" s="3" t="inlineStr">
         <is>
-          <t>P为指标实际值，0.95为目标值，0.76为底线值。
-1.若P≥0.95，得100分（满分）；
-2.若0.76&lt;P&lt;0.95，按线性比例计算，即：得分=60+(P-0.76)/(0.95-0.76)×(100-60)；
-3.若P=0.76，得60分（基础分）；
-4.若P&lt;0.76，得0分。</t>
+          <t>P为指标实际值，1为目标值，0.8为底线值。
+1.若P≥1，得100分（满分）；
+2.若0.8&lt;P&lt;1，按线性比例计算，即：得分=60+(P-0.8)/(1-0.8)×(100-60)；
+3.若P=0.8，得60分（基础分）；
+4.若P&lt;0.8，得0分。</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>人工校验</t>
+          <t>成功</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1066,21 +1066,21 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.54</t>
         </is>
       </c>
       <c r="P7" s="3" t="inlineStr">
         <is>
-          <t>P为指标实际值，0.9为目标值，0.72为底线值。
+          <t>P为指标实际值，0.9为目标值，0.54为底线值。
 1.若P≥0.9，得100分（满分）；
-2.若0.72&lt;P&lt;0.9，按线性比例计算，即：得分=60+(P-0.72)/(0.9-0.72)×(100-60)；
-3.若P=0.72，得60分（基础分）；
-4.若P&lt;0.72，得0分。</t>
+2.若0.54&lt;P&lt;0.9，按线性比例计算，即：得分=60+(P-0.54)/(0.9-0.54)×(100-60)；
+3.若P=0.54，得60分（基础分）；
+4.若P&lt;0.54，得0分。</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>人工校验</t>
+          <t>成功</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1159,26 +1159,26 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.04</t>
         </is>
       </c>
       <c r="P8" s="3" t="inlineStr">
         <is>
-          <t>P为指标实际值，0为目标值，0为底线值。
-1.若P≥0，得100分（满分）；
-2.若0&lt;P&lt;0，按线性比例计算，即：得分=60+(P-0)/(0-0)×(100-60)；
-3.若P=0，得60分（基础分）；
-4.若P&lt;0，得0分。</t>
+          <t>P为指标实际值，0为目标值，0.04为底线值。
+1.若P≤0，得100分（满分）；
+2.若0&lt;P&lt;0.04，按线性比例计算，即：得分=100-(P-0)/(0.04-0)×(100-60)；
+3.若P=0.04，得60分（基础分）；
+4.若P＞0.04，得0分。</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>人工校验</t>
+          <t>成功</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>正向</t>
+          <t>逆向</t>
         </is>
       </c>
     </row>
@@ -1248,21 +1248,21 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.18</t>
         </is>
       </c>
       <c r="P9" s="3" t="inlineStr">
         <is>
-          <t>P为指标实际值，0.25为目标值，0.2为底线值。
-1.若P≥0.25，得100分（满分）；
-2.若0.2&lt;P&lt;0.25，按线性比例计算，即：得分=60+(P-0.2)/(0.25-0.2)×(100-60)；
-3.若P=0.2，得60分（基础分）；
-4.若P&lt;0.2，得0分。</t>
+          <t>P为指标实际值，0.3为目标值，0.18为底线值。
+1.若P≥0.3，得100分（满分）；
+2.若0.18&lt;P&lt;0.3，按线性比例计算，即：得分=60+(P-0.18)/(0.3-0.18)×(100-60)；
+3.若P=0.18，得60分（基础分）；
+4.若P&lt;0.18，得0分。</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>人工校验</t>
+          <t>成功</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1337,21 +1337,21 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>0.68</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="P10" s="3" t="inlineStr">
         <is>
-          <t>P为指标实际值，0.85为目标值，0.68为底线值。
-1.若P≥0.85，得100分（满分）；
-2.若0.68&lt;P&lt;0.85，按线性比例计算，即：得分=60+(P-0.68)/(0.85-0.68)×(100-60)；
-3.若P=0.68，得60分（基础分）；
-4.若P&lt;0.68，得0分。</t>
+          <t>P为指标实际值，1为目标值，0.6为底线值。
+1.若P≥1，得100分（满分）；
+2.若0.6&lt;P&lt;1，按线性比例计算，即：得分=60+(P-0.6)/(1-0.6)×(100-60)；
+3.若P=0.6，得60分（基础分）；
+4.若P&lt;0.6，得0分。</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>人工校验</t>
+          <t>成功</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">

</xml_diff>